<commit_message>
committing all changes in preparation for making new branch and removing SA code. This is to archive software and add to thesis manuscript.
</commit_message>
<xml_diff>
--- a/lfd_package/results/helena_mt/helena_mt_results.xlsx
+++ b/lfd_package/results/helena_mt/helena_mt_results.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="helena_mt" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="pre1980_montana_helena.csv" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="pre1980_Helena_MT.csv" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="post1980_Helena_MT.csv" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2135,11 +2137,9 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>0</v>
       </c>
-      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>66816.41</v>
       </c>
@@ -3238,6 +3238,2845 @@
         <v>117</v>
       </c>
       <c r="L32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Variable Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ELF</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TLF</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr"/>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>PP Peak</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Annual Electrical Demand</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>256321.26</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Peak Electrical Demand</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>74.28</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Annual Thermal Demand</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>474408.023</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Peak Thermal Demand</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>250.755</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CHP Size</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>20.15</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>32.398</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>74.28</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TES Size</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>308.06</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>339.068</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>380.65</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Aux Boiler Size</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>250.76</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>250.76</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>250.76</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CHP Electrical Energy Generation</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>175066.34</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>175034.51</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>472449.2</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Electrical Energy Bought</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>81254.91</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>104589.86</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>48572.35</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Electrical Energy Sold</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>23303.12</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>264700.29</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CHP Thermal Energy Generation</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>327741.7</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>337383.41</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>884472.14</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TES Thermal Energy Dispatched</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>9607.98</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>37827.1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>75207.67</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Boiler Thermal Energy Generation</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>233473.69</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>140900.35</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>11624.11</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CHP Electrical Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>68.29000000000001</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>184.32</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Electricity Bought Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>18.95</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CHP Thermal Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>69.08</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>71.12</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>186.44</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TES Thermal Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>7.97</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>15.85</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Boiler Thermal Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>49.21</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>29.7</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Thermal Energy Savings</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>-335653.41</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>-219820.95</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>-1140101.3</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Electrical Energy Savings</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>437665.85</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>379328.49</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>519372.27</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Total Energy Savings</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>102012.45</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>159507.54</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>-620729.03</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Electricity Cost</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>21273.18</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>7845.03</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>9635.969999999999</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>5338.88</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Fuel Cost</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>14521.58</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>21328.26</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>18979.31</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>37641.57</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CHP Installed Cost</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>69594.06</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>111882.65</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>256529.51</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CHP O&amp;M Cost</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>5251.99</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>5251.04</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>14173.48</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TES Installed Cost</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>6457</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>7106.86</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>7978.38</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TES O&amp;M Cost</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PP Revenue</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>1787.63</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>20302.53</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Simple Payback [Yrs]</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>55.53</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>32.02</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>-250.33</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Simple Payback (37.5% incentive)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>34.71</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>20.01</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>-156.46</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CO2</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>70</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>71</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>100</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Variable Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ELF</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TLF</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr"/>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>PP Peak</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Annual Electrical Demand</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>251574.88</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Peak Electrical Demand</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>71.45999999999999</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Annual Thermal Demand</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>417064.243</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Peak Thermal Demand</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>221.049</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CHP Size</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>19.46</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>28.83</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>71.45999999999999</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TES Size</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>296.53</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>280.142</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>258.21</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Aux Boiler Size</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>221.05</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>221.05</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>221.05</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>kilowatt</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CHP Electrical Energy Generation</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>169591.18</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>155745.51</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>476414.05</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Electrical Energy Bought</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>81983.71000000001</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>108811.87</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>41398.43</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Electrical Energy Sold</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>12982.5</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>266237.6</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CHP Thermal Energy Generation</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>317491.64</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>300203.38</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>891894.74</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TES Thermal Energy Dispatched</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>8246.389999999999</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>32877.27</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>54145.55</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Boiler Thermal Energy Generation</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>187524.03</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>120205.99</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>7103.03</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CHP Electrical Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>67.41</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>61.91</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>189.37</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Electricity Bought Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>32.59</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>16.46</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CHP Thermal Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>76.13</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>71.98</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>213.85</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TES Thermal Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>7.88</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Boiler Thermal Pct Coverage</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>44.96</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>28.82</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Thermal Energy Savings</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>-329979.6</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>-195467.07</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>-1220552.24</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Electrical Energy Savings</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>423977.95</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>356907.53</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>525441.14</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Total Energy Savings</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>93998.34</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>161440.47</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>-695111.1</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>kilowatt_hour</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Electricity Cost</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>20909.19</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>7901.01</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>9959.700000000001</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>4788.56</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Fuel Cost</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>13068</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>19759.62</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>17031.85</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>37819.44</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CHP Installed Cost</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>67190.05</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>99559.8</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>246770.62</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CHP O&amp;M Cost</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>5087.74</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>4672.37</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>14292.42</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TES Installed Cost</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>6215.23</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>5871.78</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>5412.16</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TES O&amp;M Cost</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PP Revenue</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>995.91</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>20420.56</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Simple Payback [Yrs]</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>31.86</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>-100.77</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Simple Payback (37.5% incentive)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>37.33</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>19.91</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>-62.98</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>dimensionless</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CO2</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>96</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>67</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>68</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>metric_ton</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>98</v>
+      </c>
+      <c r="J32" t="inlineStr">
         <is>
           <t>metric_ton</t>
         </is>

</xml_diff>